<commit_message>
Update the width of chart
</commit_message>
<xml_diff>
--- a/ConsoleAppFSharp/Output.xlsx
+++ b/ConsoleAppFSharp/Output.xlsx
@@ -503,8 +503,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>565012</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>549459</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>166370</xdr:rowOff>
     </xdr:to>

</xml_diff>